<commit_message>
Added test unit for Database Create method
</commit_message>
<xml_diff>
--- a/BlackBox_TestCases.xlsx
+++ b/BlackBox_TestCases.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C339199-E2AF-4129-B4EA-CB2A1DC480AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5021107A-E435-4D59-AFD3-158D42874813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
-    <sheet name="Login" sheetId="1" r:id="rId2"/>
-    <sheet name="Logout" sheetId="2" r:id="rId3"/>
-    <sheet name="Registration" sheetId="3" r:id="rId4"/>
-    <sheet name="ChangePassword" sheetId="4" r:id="rId5"/>
-    <sheet name="Auth2" sheetId="5" r:id="rId6"/>
-    <sheet name="Admin" sheetId="6" r:id="rId7"/>
+    <sheet name="Database Create" sheetId="8" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="Logout" sheetId="2" r:id="rId4"/>
+    <sheet name="Registration" sheetId="3" r:id="rId5"/>
+    <sheet name="ChangePassword" sheetId="4" r:id="rId6"/>
+    <sheet name="Auth2" sheetId="5" r:id="rId7"/>
+    <sheet name="Admin" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
   <si>
     <t>Test Case</t>
   </si>
@@ -90,6 +91,12 @@
   </si>
   <si>
     <t>PDO Instance</t>
+  </si>
+  <si>
+    <t>Creates Database</t>
+  </si>
+  <si>
+    <t>No Exceptions (void)</t>
   </si>
 </sst>
 </file>
@@ -220,6 +227,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -237,12 +250,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F5AFB1-9D2E-4F13-823E-2A173F6EEB8F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,7 +599,7 @@
     <col min="6" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,6 +659,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF14DCF-5EB1-41B8-BA03-50477B8EABD9}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F56B6-00BD-4254-8A55-8196DD1212E4}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -677,7 +741,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -726,7 +790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C08B590-56A7-4A6D-BC40-CD260C7EF926}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -737,53 +801,53 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD9F26-13CD-4F24-9311-312B0105116F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -794,53 +858,53 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDFDE82-C086-4DD5-953A-CAFDB40CB8C6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -851,53 +915,53 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8FDC4F-EB20-41D0-9731-675E4B2B62B4}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -908,53 +972,53 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A573F-0C25-45C5-996C-B0109D28903D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -965,47 +1029,47 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test unit for Database CreateSuccessMsg
</commit_message>
<xml_diff>
--- a/BlackBox_TestCases.xlsx
+++ b/BlackBox_TestCases.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5021107A-E435-4D59-AFD3-158D42874813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C66B717-BE9B-4C4A-9393-A4E3F0649237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
     <sheet name="Database Create" sheetId="8" r:id="rId2"/>
-    <sheet name="Login" sheetId="1" r:id="rId3"/>
-    <sheet name="Logout" sheetId="2" r:id="rId4"/>
-    <sheet name="Registration" sheetId="3" r:id="rId5"/>
-    <sheet name="ChangePassword" sheetId="4" r:id="rId6"/>
-    <sheet name="Auth2" sheetId="5" r:id="rId7"/>
-    <sheet name="Admin" sheetId="6" r:id="rId8"/>
+    <sheet name="Database CreateSuccessMsg" sheetId="9" r:id="rId3"/>
+    <sheet name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="Logout" sheetId="2" r:id="rId5"/>
+    <sheet name="Registration" sheetId="3" r:id="rId6"/>
+    <sheet name="ChangePassword" sheetId="4" r:id="rId7"/>
+    <sheet name="Auth2" sheetId="5" r:id="rId8"/>
+    <sheet name="Admin" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="20">
   <si>
     <t>Test Case</t>
   </si>
@@ -97,6 +98,12 @@
   </si>
   <si>
     <t>No Exceptions (void)</t>
+  </si>
+  <si>
+    <t>Prints Success Message</t>
+  </si>
+  <si>
+    <t>Success Message</t>
   </si>
 </sst>
 </file>
@@ -213,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +241,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -245,11 +258,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF14DCF-5EB1-41B8-BA03-50477B8EABD9}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,6 +726,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD5C907-9920-4F81-9303-DBC1F8FF2604}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F56B6-00BD-4254-8A55-8196DD1212E4}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -790,7 +857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C08B590-56A7-4A6D-BC40-CD260C7EF926}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -801,38 +868,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -847,7 +914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD9F26-13CD-4F24-9311-312B0105116F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -858,38 +925,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -904,7 +971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDFDE82-C086-4DD5-953A-CAFDB40CB8C6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -915,38 +982,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -961,7 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8FDC4F-EB20-41D0-9731-675E4B2B62B4}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -972,38 +1039,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1018,7 +1085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A573F-0C25-45C5-996C-B0109D28903D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1029,38 +1096,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>